<commit_message>
cambios adaptacion a web
</commit_message>
<xml_diff>
--- a/public/uploads/Datos Alumnos DPW 1.xlsx
+++ b/public/uploads/Datos Alumnos DPW 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edwin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84EEEE7C-FE89-46BB-99DA-D1417492C915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3DE073C-8204-48DD-B04B-EAB0F151936E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E3E28142-02A7-4EB4-832E-BAE489A9A07C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>REGISTRO DE ESTUDIANTES</t>
   </si>
@@ -114,24 +114,6 @@
   </si>
   <si>
     <t>DISEÑO Y PROGRAMACION WEB</t>
-  </si>
-  <si>
-    <t>JORGE DAVID TUCSE ABAD</t>
-  </si>
-  <si>
-    <t>tucfseabad@GMAIL.COM</t>
-  </si>
-  <si>
-    <t>dpw75769648tucse@iestpsullana.com</t>
-  </si>
-  <si>
-    <t>I.E FE ALEGRIA</t>
-  </si>
-  <si>
-    <t>AV BUENOS AIRES</t>
-  </si>
-  <si>
-    <t>TUCSE YANAYACO JORGE</t>
   </si>
   <si>
     <t>CAMJOY AGUIREE YOYSY</t>
@@ -618,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63806873-E181-4449-B86E-CF0EAA1261E9}">
-  <dimension ref="A1:O30"/>
+  <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O12" sqref="N12:O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -630,6 +612,7 @@
     <col min="2" max="2" width="25.28515625" customWidth="1"/>
     <col min="3" max="3" width="26.7109375" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="33.7109375" customWidth="1"/>
     <col min="6" max="6" width="28.7109375" customWidth="1"/>
     <col min="7" max="7" width="44" customWidth="1"/>
     <col min="8" max="8" width="31.7109375" customWidth="1"/>
@@ -714,43 +697,43 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="C3" s="5">
-        <v>76201296</v>
+        <v>74124196</v>
       </c>
       <c r="D3" s="8">
         <v>44633</v>
       </c>
       <c r="E3" s="5">
-        <v>933826949</v>
+        <v>935295832</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>18</v>
+        <v>27</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>28</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="J3" s="6" t="s">
         <v>21</v>
       </c>
       <c r="K3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="5" t="s">
-        <v>23</v>
-      </c>
       <c r="M3" s="6" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="N3" s="5">
-        <v>972905311</v>
+        <v>985597489</v>
       </c>
       <c r="O3" s="7" t="s">
         <v>25</v>
@@ -761,94 +744,51 @@
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="C4" s="5">
-        <v>75769648</v>
+        <v>76201296</v>
       </c>
       <c r="D4" s="8">
-        <v>44634</v>
+        <v>44633</v>
       </c>
       <c r="E4" s="5">
-        <v>903564455</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>27</v>
+        <v>933826949</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>17</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="J4" s="6" t="s">
         <v>21</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L4" s="5" t="s">
         <v>23</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="N4" s="5">
-        <v>933742112</v>
+        <v>972905311</v>
       </c>
       <c r="O4" s="7" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
-        <v>3</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="5">
-        <v>74124196</v>
-      </c>
-      <c r="D5" s="8">
-        <v>44633</v>
-      </c>
-      <c r="E5" s="5">
-        <v>935295832</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="M5" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="N5" s="5">
-        <v>985597489</v>
-      </c>
-      <c r="O5" s="7" t="s">
-        <v>25</v>
-      </c>
+      <c r="L5"/>
+      <c r="M5"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L6"/>
@@ -910,9 +850,8 @@
       <c r="L20"/>
       <c r="M20"/>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="L21"/>
-      <c r="M21"/>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
@@ -934,23 +873,18 @@
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
-    </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:O1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" xr:uid="{C824068E-4080-48C5-9152-00FE9DB1D620}"/>
-    <hyperlink ref="G3" r:id="rId2" xr:uid="{A2287EED-698B-4E11-A212-4CC45B974F40}"/>
-    <hyperlink ref="F4" r:id="rId3" xr:uid="{0CF47BE9-8041-4100-B3E4-67B320A364C1}"/>
-    <hyperlink ref="G4" r:id="rId4" xr:uid="{ADEA0132-8047-4A0C-AC63-7A441FB4B0EE}"/>
-    <hyperlink ref="F5" r:id="rId5" xr:uid="{9763C259-0B71-4B29-9A76-C516D849D7E0}"/>
-    <hyperlink ref="G5" r:id="rId6" xr:uid="{D4474C33-2275-4FF8-915F-45514D4655EC}"/>
+    <hyperlink ref="F4" r:id="rId1" xr:uid="{E972E397-32CD-4C1F-9265-133DDC68D402}"/>
+    <hyperlink ref="G4" r:id="rId2" xr:uid="{B32D829E-D3AF-4436-87A4-BD654C90376B}"/>
+    <hyperlink ref="F3" r:id="rId3" xr:uid="{A0A1788E-6F28-4A95-BB0F-4DFDE5FE2844}"/>
+    <hyperlink ref="G3" r:id="rId4" xr:uid="{CC315858-4228-4289-B45F-CABA18CFD552}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>